<commit_message>
added results and updated tests
</commit_message>
<xml_diff>
--- a/src/opt/test/Adult_RHC_Restarts_Results.xlsx
+++ b/src/opt/test/Adult_RHC_Restarts_Results.xlsx
@@ -5,17 +5,31 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jrafferty3\Dropbox\GradSchool\Machine Learning\StolenCode\CS4641-Machine-Learning\2. Randomized Optimization\ABAGAIL\src\opt\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jrafferty3\Documents\School\ML\CS7641\Randomized Optimization\ABAGAIL\src\opt\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21075" windowHeight="11580"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Adult_RHC_Restarts_Results" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Iterations</t>
+  </si>
+  <si>
+    <t>Train Error</t>
+  </si>
+  <si>
+    <t>Test Error</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -572,6 +586,45 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Randomized</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Hill Climbing</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Error vs. Number of Restarts</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -610,8 +663,19 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Adult_RHC_Restarts_Results!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Train Error</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -624,55 +688,111 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Adult_RHC_Restarts_Results!$B$1:$B$10</c:f>
+              <c:f>Adult_RHC_Restarts_Results!$B$2:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>6.7842516975263806E-2</c:v>
+                  <c:v>0.10397498853268899</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.6725024238992005E-2</c:v>
+                  <c:v>9.1827106684920404E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.4972135126796794E-2</c:v>
+                  <c:v>0.10301032416334099</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.10167045635896101</c:v>
+                  <c:v>0.20314481579336399</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.0977281627194105E-2</c:v>
+                  <c:v>0.19128017690309801</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.10272891231698</c:v>
+                  <c:v>9.8403261033289405E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.13099190360509599</c:v>
+                  <c:v>0.17653608047378899</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.105656254902735</c:v>
+                  <c:v>9.3628939385494894E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.0492516061184105E-2</c:v>
+                  <c:v>0.137834740104093</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.9785058972622997E-2</c:v>
+                  <c:v>0.16968938013403001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.12909332226547399</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.15871804651489499</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.61858222828334E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.18128929330943799</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.172704503919547</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.111527601172468</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.181408428545098</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.19556690086505801</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.13451794222867</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.137139468521942</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.12652067875957701</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.13010342537090699</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.15544827404320199</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.100830694736152</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.19838213553978001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A0E2-4B6A-A30D-0618B7281434}"/>
+              <c16:uniqueId val="{00000001-CF3C-4CCB-B616-EFB93B9FE4D7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Adult_RHC_Restarts_Results!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Test Error</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:schemeClr val="accent4"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -682,50 +802,96 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Adult_RHC_Restarts_Results!$C$1:$C$10</c:f>
+              <c:f>Adult_RHC_Restarts_Results!$C$2:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>2.8884721658226399E-2</c:v>
+                  <c:v>0.10369621345754</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.7157708822416501E-2</c:v>
+                  <c:v>9.1779423776261304E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0831174490348003E-2</c:v>
+                  <c:v>0.104049726894682</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.3769108286514799E-2</c:v>
+                  <c:v>0.20221583998865</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.0454127484150401E-2</c:v>
+                  <c:v>0.19307806633879401</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.4102022417358097E-2</c:v>
+                  <c:v>9.8674149922587204E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.5734882485019802E-2</c:v>
+                  <c:v>0.176504520093518</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.5402387145614002E-2</c:v>
+                  <c:v>9.1051008591772495E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.0422430428730898E-2</c:v>
+                  <c:v>0.13791656279026401</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.8481105016818999E-2</c:v>
+                  <c:v>0.16988981076151299</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.12918007659067901</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.15915490810492</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.5483994923655197E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.181426507397733</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.17204348471703201</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.111631591354037</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.18023446599812201</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.194665463370638</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.134323157988255</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.13730340911064501</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.12666910056266201</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.13001432463316201</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.154538858097205</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.100423301232955</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.198392396161615</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-A0E2-4B6A-A30D-0618B7281434}"/>
+              <c16:uniqueId val="{00000000-E734-462F-BB64-A7AD6FE675E5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -735,16 +901,210 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="802271135"/>
-        <c:axId val="802271551"/>
+        <c:axId val="814879039"/>
+        <c:axId val="814889855"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Adult_RHC_Restarts_Results!$A$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Iterations</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Adult_RHC_Restarts_Results!$A$2:$A$26</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="25"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>23</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>25</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-CF3C-4CCB-B616-EFB93B9FE4D7}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="802271135"/>
+        <c:axId val="814879039"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of Restarts</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -781,7 +1141,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="802271551"/>
+        <c:crossAx val="814889855"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -789,10 +1149,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="802271551"/>
+        <c:axId val="814889855"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.16000000000000003"/>
+          <c:max val="0.21000000000000002"/>
+          <c:min val="5.000000000000001E-2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -810,6 +1171,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Error</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -817,7 +1234,9 @@
         <c:spPr>
           <a:noFill/>
           <a:ln>
-            <a:noFill/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -841,11 +1260,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="802271135"/>
+        <c:crossAx val="814879039"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="4.0000000000000008E-2"/>
-        <c:minorUnit val="8.0000000000000019E-3"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1472,15 +1889,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>357187</xdr:colOff>
+      <xdr:colOff>361949</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:rowOff>95249</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
+      <xdr:colOff>142874</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1765,23 +2182,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W23" sqref="W23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>6.7842516975263806E-2</v>
-      </c>
-      <c r="C1">
-        <v>2.8884721658226399E-2</v>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1789,10 +2206,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>8.6725024238992005E-2</v>
+        <v>0.10397498853268899</v>
       </c>
       <c r="C2">
-        <v>3.7157708822416501E-2</v>
+        <v>0.10369621345754</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1800,10 +2217,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>9.4972135126796794E-2</v>
+        <v>9.1827106684920404E-2</v>
       </c>
       <c r="C3">
-        <v>4.0831174490348003E-2</v>
+        <v>9.1779423776261304E-2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1811,10 +2228,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.10167045635896101</v>
+        <v>0.10301032416334099</v>
       </c>
       <c r="C4">
-        <v>4.3769108286514799E-2</v>
+        <v>0.104049726894682</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1822,10 +2239,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>7.0977281627194105E-2</v>
+        <v>0.20314481579336399</v>
       </c>
       <c r="C5">
-        <v>3.0454127484150401E-2</v>
+        <v>0.20221583998865</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1833,10 +2250,10 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.10272891231698</v>
+        <v>0.19128017690309801</v>
       </c>
       <c r="C6">
-        <v>4.4102022417358097E-2</v>
+        <v>0.19307806633879401</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1844,10 +2261,10 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0.13099190360509599</v>
+        <v>9.8403261033289405E-2</v>
       </c>
       <c r="C7">
-        <v>5.5734882485019802E-2</v>
+        <v>9.8674149922587204E-2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1855,10 +2272,10 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0.105656254902735</v>
+        <v>0.17653608047378899</v>
       </c>
       <c r="C8">
-        <v>4.5402387145614002E-2</v>
+        <v>0.176504520093518</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1866,10 +2283,10 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>7.0492516061184105E-2</v>
+        <v>9.3628939385494894E-2</v>
       </c>
       <c r="C9">
-        <v>3.0422430428730898E-2</v>
+        <v>9.1051008591772495E-2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1877,10 +2294,10 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>8.9785058972622997E-2</v>
+        <v>0.137834740104093</v>
       </c>
       <c r="C10">
-        <v>3.8481105016818999E-2</v>
+        <v>0.13791656279026401</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1888,10 +2305,10 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>7.9374475414369594E-2</v>
+        <v>0.16968938013403001</v>
       </c>
       <c r="C11">
-        <v>3.40479983835855E-2</v>
+        <v>0.16988981076151299</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1899,10 +2316,10 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>8.0689875837388902E-2</v>
+        <v>0.12909332226547399</v>
       </c>
       <c r="C12">
-        <v>3.4609278940735198E-2</v>
+        <v>0.12918007659067901</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1910,10 +2327,10 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>6.5051632857757294E-2</v>
+        <v>0.15871804651489499</v>
       </c>
       <c r="C13">
-        <v>2.7733387770476001E-2</v>
+        <v>0.15915490810492</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1921,10 +2338,10 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>9.6482864723422407E-2</v>
+        <v>9.61858222828334E-2</v>
       </c>
       <c r="C14">
-        <v>4.1313359377073602E-2</v>
+        <v>9.5483994923655197E-2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1932,10 +2349,10 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>7.9050919532277303E-2</v>
+        <v>0.18128929330943799</v>
       </c>
       <c r="C15">
-        <v>3.3956403050486597E-2</v>
+        <v>0.181426507397733</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1943,10 +2360,10 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>0.11536097394193399</v>
+        <v>0.172704503919547</v>
       </c>
       <c r="C16">
-        <v>4.9604655728638099E-2</v>
+        <v>0.17204348471703201</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1954,10 +2371,10 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>0.14861959591613799</v>
+        <v>0.111527601172468</v>
       </c>
       <c r="C17">
-        <v>6.3946324357079601E-2</v>
+        <v>0.111631591354037</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1965,10 +2382,10 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>6.8076500549565003E-2</v>
+        <v>0.181408428545098</v>
       </c>
       <c r="C18">
-        <v>2.8962243331083899E-2</v>
+        <v>0.18023446599812201</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1976,10 +2393,10 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>8.1361879497584499E-2</v>
+        <v>0.19556690086505801</v>
       </c>
       <c r="C19">
-        <v>3.4853174790549099E-2</v>
+        <v>0.194665463370638</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1987,10 +2404,10 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>0.15538531509741799</v>
+        <v>0.13451794222867</v>
       </c>
       <c r="C20">
-        <v>6.6627492130836102E-2</v>
+        <v>0.134323157988255</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1998,10 +2415,10 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>7.5654465346743902E-2</v>
+        <v>0.137139468521942</v>
       </c>
       <c r="C21">
-        <v>3.21991854292112E-2</v>
+        <v>0.13730340911064501</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2009,10 +2426,10 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>7.0592951076614105E-2</v>
+        <v>0.12652067875957701</v>
       </c>
       <c r="C22">
-        <v>3.0014517062431301E-2</v>
+        <v>0.12666910056266201</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2020,10 +2437,10 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>9.3052658886841305E-2</v>
+        <v>0.13010342537090699</v>
       </c>
       <c r="C23">
-        <v>3.9924478331328901E-2</v>
+        <v>0.13001432463316201</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2031,10 +2448,10 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>0.118553095321332</v>
+        <v>0.15544827404320199</v>
       </c>
       <c r="C24">
-        <v>5.0363038206693203E-2</v>
+        <v>0.154538858097205</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2042,14 +2459,26 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>0.11155368426022801</v>
+        <v>0.100830694736152</v>
       </c>
       <c r="C25">
-        <v>4.7646908838397499E-2</v>
+        <v>0.100423301232955</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>0.19838213553978001</v>
+      </c>
+      <c r="C26">
+        <v>0.198392396161615</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>